<commit_message>
Correçao de bugs em CP e Reatores.
</commit_message>
<xml_diff>
--- a/Resultados/Resultado FuseIn.xlsx
+++ b/Resultados/Resultado FuseIn.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>37.68844221105527</v>
+        <v>25.12562814070353</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12.5592585329202</v>
+        <v>8.372839021946804</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>300</v>
+        <v>200.0000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7957747154594768</v>
+        <v>0.5305164769729848</v>
       </c>
     </row>
     <row r="9">
@@ -678,46 +678,46 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2</v>
+        <v>0.31</v>
       </c>
       <c r="D2" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E2" t="n">
-        <v>28</v>
+        <v>24.5</v>
       </c>
       <c r="F2" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" t="n">
-        <v>45.39317073170731</v>
+        <v>35.88039215686275</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9883332747654354</v>
+        <v>0.7629239313978801</v>
       </c>
       <c r="I2" t="n">
-        <v>1.55309514605997</v>
+        <v>1.183310587474263</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9130580458563072</v>
+        <v>0.8400962150695708</v>
       </c>
       <c r="K2" t="n">
-        <v>0.08088495240019192</v>
+        <v>0.04878205554956144</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9883332747654354</v>
+        <v>0.7629239313978801</v>
       </c>
       <c r="M2" t="n">
-        <v>2.084171873822439</v>
+        <v>1.397935380692977</v>
       </c>
       <c r="N2" t="n">
-        <v>45.39317073170731</v>
+        <v>35.88039215686275</v>
       </c>
       <c r="O2" t="n">
-        <v>8.914044183731294</v>
+        <v>10.72470940855171</v>
       </c>
     </row>
   </sheetData>
@@ -731,7 +731,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,16 +782,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>3.141110748710648</v>
+        <v>2.284444180880472</v>
       </c>
       <c r="E2" t="n">
-        <v>0.112182526739666</v>
+        <v>0.09324261962777437</v>
       </c>
       <c r="F2" t="n">
-        <v>2.084171873822439</v>
+        <v>1.397935380692977</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2921785746740184</v>
+        <v>0.2688307888222627</v>
       </c>
     </row>
     <row r="3">
@@ -799,22 +799,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.005988023952096</v>
+        <v>1.006578947368421</v>
       </c>
       <c r="C3" t="n">
-        <v>1.077844311377246</v>
+        <v>1.085526315789474</v>
       </c>
       <c r="D3" t="n">
-        <v>3.385628351903693</v>
+        <v>2.47982427529788</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1209152982822748</v>
+        <v>0.1012173173590972</v>
       </c>
       <c r="F3" t="n">
-        <v>2.20116659588326</v>
+        <v>1.482553309618666</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3394379798285418</v>
+        <v>0.3167814328984634</v>
       </c>
     </row>
     <row r="4">
@@ -822,22 +822,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.012987012987013</v>
+        <v>1.014388489208633</v>
       </c>
       <c r="C4" t="n">
-        <v>1.168831168831169</v>
+        <v>1.18705035971223</v>
       </c>
       <c r="D4" t="n">
-        <v>3.671428147843613</v>
+        <v>2.711750286656675</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1311224338515576</v>
+        <v>0.1106836851696602</v>
       </c>
       <c r="F4" t="n">
-        <v>2.329629856355598</v>
+        <v>1.575851798120855</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3991645226614181</v>
+        <v>0.3788063881624192</v>
       </c>
     </row>
     <row r="5">
@@ -845,22 +845,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.021276595744681</v>
+        <v>1.023809523809524</v>
       </c>
       <c r="C5" t="n">
-        <v>1.276595744680851</v>
+        <v>1.309523809523809</v>
       </c>
       <c r="D5" t="n">
-        <v>4.009928615375296</v>
+        <v>2.991534046391093</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1432117362634034</v>
+        <v>0.1221034304649426</v>
       </c>
       <c r="F5" t="n">
-        <v>2.470231283842391</v>
+        <v>1.678077193093751</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4761624575945977</v>
+        <v>0.4610051792445262</v>
       </c>
     </row>
     <row r="6">
@@ -868,22 +868,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.03125</v>
+        <v>1.035398230088496</v>
       </c>
       <c r="C6" t="n">
-        <v>1.40625</v>
+        <v>1.460176991150443</v>
       </c>
       <c r="D6" t="n">
-        <v>4.417186990374349</v>
+        <v>3.335692830489185</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1577566782276553</v>
+        <v>0.1361507277750688</v>
       </c>
       <c r="F6" t="n">
-        <v>2.622792641284897</v>
+        <v>1.788336944445124</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5777945446434447</v>
+        <v>0.5731786534330099</v>
       </c>
     </row>
     <row r="7">
@@ -891,22 +891,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.043478260869566</v>
+        <v>1.05</v>
       </c>
       <c r="C7" t="n">
-        <v>1.565217391304348</v>
+        <v>1.65</v>
       </c>
       <c r="D7" t="n">
-        <v>4.916521171894928</v>
+        <v>3.769332898452778</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1755900418533903</v>
+        <v>0.1538503223858277</v>
       </c>
       <c r="F7" t="n">
-        <v>2.785104054106082</v>
+        <v>1.902939536968315</v>
       </c>
       <c r="G7" t="n">
-        <v>0.7158098918289754</v>
+        <v>0.7318918225686103</v>
       </c>
     </row>
     <row r="8">
@@ -914,22 +914,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1.058823529411765</v>
+        <v>1.068965517241379</v>
       </c>
       <c r="C8" t="n">
-        <v>1.764705882352942</v>
+        <v>1.896551724137931</v>
       </c>
       <c r="D8" t="n">
-        <v>5.543136615371733</v>
+        <v>4.332566549945723</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1979691648347047</v>
+        <v>0.1768394510181928</v>
       </c>
       <c r="F8" t="n">
-        <v>2.950227565964447</v>
+        <v>2.01129822905886</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9098986754554209</v>
+        <v>0.9669597338731801</v>
       </c>
     </row>
     <row r="9">
@@ -937,22 +937,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1.078651685393258</v>
+        <v>1.094594594594595</v>
       </c>
       <c r="C9" t="n">
-        <v>2.022471910112359</v>
+        <v>2.22972972972973</v>
       </c>
       <c r="D9" t="n">
-        <v>4.681016609551054</v>
+        <v>5.093693106017269</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1671791646268233</v>
+        <v>0.2079058410619293</v>
       </c>
       <c r="F9" t="n">
-        <v>2.086558351937485</v>
+        <v>2.085032363369227</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4668287239314098</v>
+        <v>1.336544599285263</v>
       </c>
     </row>
     <row r="10">
@@ -960,22 +960,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1.105263157894737</v>
+        <v>1.131147540983607</v>
       </c>
       <c r="C10" t="n">
-        <v>2.36842105263158</v>
+        <v>2.704918032786887</v>
       </c>
       <c r="D10" t="n">
-        <v>5.481716819079525</v>
+        <v>2.284444180880472</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1957756006814116</v>
+        <v>0.09324261962777437</v>
       </c>
       <c r="F10" t="n">
-        <v>2.146073671965481</v>
+        <v>1.397935380692977</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6401922303082929</v>
+        <v>1.344153944111314</v>
       </c>
     </row>
     <row r="11">
@@ -983,45 +983,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1.142857142857143</v>
+        <v>1.1875</v>
       </c>
       <c r="C11" t="n">
-        <v>2.857142857142857</v>
+        <v>3.4375</v>
       </c>
       <c r="D11" t="n">
-        <v>3.141110748710648</v>
+        <v>2.284444180880472</v>
       </c>
       <c r="E11" t="n">
-        <v>0.112182526739666</v>
+        <v>0.09324261962777437</v>
       </c>
       <c r="F11" t="n">
-        <v>2.084171873822439</v>
+        <v>1.397935380692977</v>
       </c>
       <c r="G11" t="n">
-        <v>1.606982160707101</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="C12" t="n">
-        <v>3.600000000000001</v>
-      </c>
-      <c r="D12" t="n">
-        <v>3.141110748710648</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.112182526739666</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2.084171873822439</v>
-      </c>
-      <c r="G12" t="n">
-        <v>3.213964321414202</v>
+        <v>2.688307888222627</v>
       </c>
     </row>
   </sheetData>

</xml_diff>